<commit_message>
Added game data for april 1, 2025 - april 3, 2025
</commit_message>
<xml_diff>
--- a/data/processed/nba_points_2024_2025.xlsx
+++ b/data/processed/nba_points_2024_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA70C65-E572-3447-976A-7C4FD411E479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFA7929-00EE-3445-9DD3-00F1AE30E475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6796" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6928" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -1028,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y1130"/>
+  <dimension ref="A1:Y1152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1131" sqref="A1131"/>
+      <pane ySplit="1" topLeftCell="A1128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q1140" sqref="Q1140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1207,15 +1207,15 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>1122</v>
+        <v>1144</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>583</v>
+        <v>595</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>537</v>
+        <v>547</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
@@ -1370,15 +1370,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.51960784313725494</v>
+        <v>0.5201048951048951</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.47860962566844922</v>
+        <v>0.47814685314685312</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>4.4563279857397506E-3</v>
+        <v>4.370629370629371E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1526,11 +1526,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>14.910806174957118</v>
+        <v>14.920168067226891</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>14.62290502793296</v>
+        <v>14.564899451553931</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -62542,34 +62542,34 @@
         <v>106</v>
       </c>
       <c r="M892" s="30">
-        <f t="shared" ref="M892:M1130" si="42">K892+L892</f>
+        <f t="shared" ref="M892:M1146" si="42">K892+L892</f>
         <v>208</v>
       </c>
       <c r="N892" s="30">
-        <f t="shared" ref="N892:N1130" si="43">(L892-K892)*-1</f>
+        <f t="shared" ref="N892:N1146" si="43">(L892-K892)*-1</f>
         <v>-4</v>
       </c>
       <c r="O892" s="30">
         <v>1</v>
       </c>
       <c r="P892" s="30">
-        <f t="shared" ref="P892:P1130" si="44">IF(M892&gt;I892,1,0)</f>
+        <f t="shared" ref="P892:P1146" si="44">IF(M892&gt;I892,1,0)</f>
         <v>0</v>
       </c>
       <c r="Q892" s="30" t="str">
-        <f t="shared" ref="Q892:Q1130" si="45">IF(P892=1,(M892-I892), "")</f>
+        <f t="shared" ref="Q892:Q1146" si="45">IF(P892=1,(M892-I892), "")</f>
         <v/>
       </c>
       <c r="R892" s="30">
-        <f t="shared" ref="R892:R1130" si="46">IF(M892&lt;I892, 1, 0)</f>
+        <f t="shared" ref="R892:R1146" si="46">IF(M892&lt;I892, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S892" s="30">
-        <f t="shared" ref="S892:S1130" si="47">IF(R892=1,(I892-M892),"")</f>
+        <f t="shared" ref="S892:S1146" si="47">IF(R892=1,(I892-M892),"")</f>
         <v>13.5</v>
       </c>
       <c r="T892" s="30">
-        <f t="shared" ref="T892:T1130" si="48">IF(M892=I892,1,0)</f>
+        <f t="shared" ref="T892:T1146" si="48">IF(M892=I892,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -78992,6 +78992,1524 @@
       </c>
       <c r="T1130" s="10">
         <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1131" s="29">
+        <v>45748</v>
+      </c>
+      <c r="B1131" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1131" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1131" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1131" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1131" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1131" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1131" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1131" s="30">
+        <v>224.5</v>
+      </c>
+      <c r="J1131" s="31">
+        <v>-14</v>
+      </c>
+      <c r="K1131" s="30">
+        <v>91</v>
+      </c>
+      <c r="L1131" s="30">
+        <v>105</v>
+      </c>
+      <c r="M1131" s="30">
+        <f t="shared" si="42"/>
+        <v>196</v>
+      </c>
+      <c r="N1131" s="30">
+        <f t="shared" si="43"/>
+        <v>-14</v>
+      </c>
+      <c r="O1131" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1131" s="30">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q1131" s="30" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R1131" s="30">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S1131" s="30">
+        <f t="shared" si="47"/>
+        <v>28.5</v>
+      </c>
+      <c r="T1131" s="30">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1132" s="29">
+        <v>45748</v>
+      </c>
+      <c r="B1132" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1132" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1132" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1132" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1132" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1132" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1132" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1132" s="30">
+        <v>237.5</v>
+      </c>
+      <c r="J1132" s="31">
+        <v>-6.5</v>
+      </c>
+      <c r="K1132" s="30">
+        <v>127</v>
+      </c>
+      <c r="L1132" s="30">
+        <v>113</v>
+      </c>
+      <c r="M1132" s="30">
+        <f t="shared" si="42"/>
+        <v>240</v>
+      </c>
+      <c r="N1132" s="30">
+        <f t="shared" si="43"/>
+        <v>14</v>
+      </c>
+      <c r="O1132" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1132" s="30">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1132" s="30">
+        <f t="shared" si="45"/>
+        <v>2.5</v>
+      </c>
+      <c r="R1132" s="30">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1132" s="30" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1132" s="30">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1133" s="29">
+        <v>45748</v>
+      </c>
+      <c r="B1133" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1133" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1133" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1133" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1133" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1133" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1133" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1133" s="30">
+        <v>220.5</v>
+      </c>
+      <c r="J1133" s="31">
+        <v>-6.5</v>
+      </c>
+      <c r="K1133" s="30">
+        <v>123</v>
+      </c>
+      <c r="L1133" s="30">
+        <v>133</v>
+      </c>
+      <c r="M1133" s="30">
+        <f t="shared" si="42"/>
+        <v>256</v>
+      </c>
+      <c r="N1133" s="30">
+        <f t="shared" si="43"/>
+        <v>-10</v>
+      </c>
+      <c r="O1133" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1133" s="30">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1133" s="30">
+        <f t="shared" si="45"/>
+        <v>35.5</v>
+      </c>
+      <c r="R1133" s="30">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1133" s="30" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1133" s="30">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1134" s="29">
+        <v>45748</v>
+      </c>
+      <c r="B1134" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1134" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1134" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1134" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1134" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1134" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1134" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1134" s="30">
+        <v>218.5</v>
+      </c>
+      <c r="J1134" s="31">
+        <v>4</v>
+      </c>
+      <c r="K1134" s="30">
+        <v>116</v>
+      </c>
+      <c r="L1134" s="30">
+        <v>105</v>
+      </c>
+      <c r="M1134" s="30">
+        <f t="shared" si="42"/>
+        <v>221</v>
+      </c>
+      <c r="N1134" s="30">
+        <f t="shared" si="43"/>
+        <v>11</v>
+      </c>
+      <c r="O1134" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1134" s="30">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1134" s="30">
+        <f t="shared" si="45"/>
+        <v>2.5</v>
+      </c>
+      <c r="R1134" s="30">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1134" s="30" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1134" s="30">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1135" s="29">
+        <v>45748</v>
+      </c>
+      <c r="B1135" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1135" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1135" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1135" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1135" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1135" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1135" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1135" s="30">
+        <v>237.5</v>
+      </c>
+      <c r="J1135" s="31">
+        <v>2.5</v>
+      </c>
+      <c r="K1135" s="30">
+        <v>134</v>
+      </c>
+      <c r="L1135" s="30">
+        <v>125</v>
+      </c>
+      <c r="M1135" s="30">
+        <f t="shared" si="42"/>
+        <v>259</v>
+      </c>
+      <c r="N1135" s="30">
+        <f t="shared" si="43"/>
+        <v>9</v>
+      </c>
+      <c r="O1135" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1135" s="30">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1135" s="30">
+        <f t="shared" si="45"/>
+        <v>21.5</v>
+      </c>
+      <c r="R1135" s="30">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1135" s="30" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1135" s="30">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1136" s="29">
+        <v>45748</v>
+      </c>
+      <c r="B1136" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1136" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1136" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1136" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1136" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1136" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1136" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1136" s="30">
+        <v>239.5</v>
+      </c>
+      <c r="J1136" s="31">
+        <v>-5.5</v>
+      </c>
+      <c r="K1136" s="30">
+        <v>118</v>
+      </c>
+      <c r="L1136" s="30">
+        <v>137</v>
+      </c>
+      <c r="M1136" s="30">
+        <f t="shared" si="42"/>
+        <v>255</v>
+      </c>
+      <c r="N1136" s="30">
+        <f t="shared" si="43"/>
+        <v>-19</v>
+      </c>
+      <c r="O1136" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1136" s="30">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1136" s="30">
+        <f t="shared" si="45"/>
+        <v>15.5</v>
+      </c>
+      <c r="R1136" s="30">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1136" s="30" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1136" s="30">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1137" s="29">
+        <v>45748</v>
+      </c>
+      <c r="B1137" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1137" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1137" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1137" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1137" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1137" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1137" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1137" s="30">
+        <v>230.5</v>
+      </c>
+      <c r="J1137" s="31">
+        <v>-2</v>
+      </c>
+      <c r="K1137" s="30">
+        <v>140</v>
+      </c>
+      <c r="L1137" s="30">
+        <v>139</v>
+      </c>
+      <c r="M1137" s="30">
+        <f t="shared" si="42"/>
+        <v>279</v>
+      </c>
+      <c r="N1137" s="30">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="O1137" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1137" s="30">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1137" s="30">
+        <f t="shared" si="45"/>
+        <v>48.5</v>
+      </c>
+      <c r="R1137" s="30">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1137" s="30" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1137" s="30">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1138" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1138" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1138" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1138" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1138" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1138" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1138" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1138" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1138" s="10">
+        <v>231.5</v>
+      </c>
+      <c r="J1138" s="11">
+        <v>-10.5</v>
+      </c>
+      <c r="K1138" s="10">
+        <v>105</v>
+      </c>
+      <c r="L1138" s="10">
+        <v>124</v>
+      </c>
+      <c r="M1138" s="10">
+        <f t="shared" si="42"/>
+        <v>229</v>
+      </c>
+      <c r="N1138" s="10">
+        <f t="shared" si="43"/>
+        <v>-19</v>
+      </c>
+      <c r="O1138" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1138" s="10">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q1138" s="10" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R1138" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S1138" s="10">
+        <f t="shared" si="47"/>
+        <v>2.5</v>
+      </c>
+      <c r="T1138" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1139" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1139" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1139" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1139" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1139" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1139" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1139" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1139" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1139" s="10">
+        <v>223.5</v>
+      </c>
+      <c r="J1139" s="11">
+        <v>-14.5</v>
+      </c>
+      <c r="K1139" s="10">
+        <v>105</v>
+      </c>
+      <c r="L1139" s="10">
+        <v>119</v>
+      </c>
+      <c r="M1139" s="10">
+        <f t="shared" si="42"/>
+        <v>224</v>
+      </c>
+      <c r="N1139" s="10">
+        <f t="shared" si="43"/>
+        <v>-14</v>
+      </c>
+      <c r="O1139" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1139" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1139" s="10">
+        <f t="shared" si="45"/>
+        <v>0.5</v>
+      </c>
+      <c r="R1139" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1139" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1139" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1140" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1140" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1140" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1140" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1140" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1140" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1140" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1140" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1140" s="10">
+        <v>230.5</v>
+      </c>
+      <c r="J1140" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="K1140" s="10">
+        <v>111</v>
+      </c>
+      <c r="L1140" s="10">
+        <v>116</v>
+      </c>
+      <c r="M1140" s="10">
+        <f t="shared" si="42"/>
+        <v>227</v>
+      </c>
+      <c r="N1140" s="10">
+        <f t="shared" si="43"/>
+        <v>-5</v>
+      </c>
+      <c r="O1140" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1140" s="10">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q1140" s="10" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R1140" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S1140" s="10">
+        <f t="shared" si="47"/>
+        <v>3.5</v>
+      </c>
+      <c r="T1140" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1141" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1141" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1141" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1141" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1141" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1141" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1141" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1141" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1141" s="10">
+        <v>212.5</v>
+      </c>
+      <c r="J1141" s="11">
+        <v>-10.5</v>
+      </c>
+      <c r="K1141" s="10">
+        <v>124</v>
+      </c>
+      <c r="L1141" s="10">
+        <v>103</v>
+      </c>
+      <c r="M1141" s="10">
+        <f t="shared" si="42"/>
+        <v>227</v>
+      </c>
+      <c r="N1141" s="10">
+        <f t="shared" si="43"/>
+        <v>21</v>
+      </c>
+      <c r="O1141" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1141" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1141" s="10">
+        <f t="shared" si="45"/>
+        <v>14.5</v>
+      </c>
+      <c r="R1141" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1141" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1141" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1142" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1142" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1142" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1142" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1142" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1142" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1142" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1142" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1142" s="10">
+        <v>227.5</v>
+      </c>
+      <c r="J1142" s="11">
+        <v>-17.5</v>
+      </c>
+      <c r="K1142" s="10">
+        <v>105</v>
+      </c>
+      <c r="L1142" s="10">
+        <v>143</v>
+      </c>
+      <c r="M1142" s="10">
+        <f t="shared" si="42"/>
+        <v>248</v>
+      </c>
+      <c r="N1142" s="10">
+        <f t="shared" si="43"/>
+        <v>-38</v>
+      </c>
+      <c r="O1142" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1142" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1142" s="10">
+        <f t="shared" si="45"/>
+        <v>20.5</v>
+      </c>
+      <c r="R1142" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1142" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1142" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1143" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1143" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1143" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1143" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1143" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1143" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1143" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1143" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1143" s="10">
+        <v>237.5</v>
+      </c>
+      <c r="J1143" s="11">
+        <v>-2.5</v>
+      </c>
+      <c r="K1143" s="10">
+        <v>118</v>
+      </c>
+      <c r="L1143" s="10">
+        <v>120</v>
+      </c>
+      <c r="M1143" s="10">
+        <f t="shared" si="42"/>
+        <v>238</v>
+      </c>
+      <c r="N1143" s="10">
+        <f t="shared" si="43"/>
+        <v>-2</v>
+      </c>
+      <c r="O1143" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1143" s="10">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="Q1143" s="10">
+        <f t="shared" si="45"/>
+        <v>0.5</v>
+      </c>
+      <c r="R1143" s="10">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="S1143" s="10" t="str">
+        <f t="shared" si="47"/>
+        <v/>
+      </c>
+      <c r="T1143" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1144" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1144" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1144" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1144" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1144" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1144" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1144" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1144" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1144" s="10">
+        <v>235.5</v>
+      </c>
+      <c r="J1144" s="11">
+        <v>-13.5</v>
+      </c>
+      <c r="K1144" s="10">
+        <v>113</v>
+      </c>
+      <c r="L1144" s="10">
+        <v>106</v>
+      </c>
+      <c r="M1144" s="10">
+        <f t="shared" si="42"/>
+        <v>219</v>
+      </c>
+      <c r="N1144" s="10">
+        <f t="shared" si="43"/>
+        <v>7</v>
+      </c>
+      <c r="O1144" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1144" s="10">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q1144" s="10" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R1144" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S1144" s="10">
+        <f t="shared" si="47"/>
+        <v>16.5</v>
+      </c>
+      <c r="T1144" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1145" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1145" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1145" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1145" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1145" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1145" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1145" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1145" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1145" s="10">
+        <v>228.5</v>
+      </c>
+      <c r="J1145" s="11">
+        <v>-13.5</v>
+      </c>
+      <c r="K1145" s="10">
+        <v>103</v>
+      </c>
+      <c r="L1145" s="10">
+        <v>119</v>
+      </c>
+      <c r="M1145" s="10">
+        <f t="shared" si="42"/>
+        <v>222</v>
+      </c>
+      <c r="N1145" s="10">
+        <f t="shared" si="43"/>
+        <v>-16</v>
+      </c>
+      <c r="O1145" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1145" s="10">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q1145" s="10" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R1145" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S1145" s="10">
+        <f t="shared" si="47"/>
+        <v>6.5</v>
+      </c>
+      <c r="T1145" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1146" s="9">
+        <v>45749</v>
+      </c>
+      <c r="B1146" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1146" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1146" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1146" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1146" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1146" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1146" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1146" s="10">
+        <v>217.5</v>
+      </c>
+      <c r="J1146" s="11">
+        <v>-17.5</v>
+      </c>
+      <c r="K1146" s="10">
+        <v>98</v>
+      </c>
+      <c r="L1146" s="10">
+        <v>114</v>
+      </c>
+      <c r="M1146" s="10">
+        <f t="shared" si="42"/>
+        <v>212</v>
+      </c>
+      <c r="N1146" s="10">
+        <f t="shared" si="43"/>
+        <v>-16</v>
+      </c>
+      <c r="O1146" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1146" s="10">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="Q1146" s="10" t="str">
+        <f t="shared" si="45"/>
+        <v/>
+      </c>
+      <c r="R1146" s="10">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="S1146" s="10">
+        <f t="shared" si="47"/>
+        <v>5.5</v>
+      </c>
+      <c r="T1146" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1147" s="29">
+        <v>45750</v>
+      </c>
+      <c r="B1147" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1147" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1147" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1147" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1147" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1147" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1147" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1147" s="30">
+        <v>216.5</v>
+      </c>
+      <c r="J1147" s="31">
+        <v>13.5</v>
+      </c>
+      <c r="K1147" s="30">
+        <v>109</v>
+      </c>
+      <c r="L1147" s="30">
+        <v>97</v>
+      </c>
+      <c r="M1147" s="30">
+        <f t="shared" ref="M1147:M1152" si="49">K1147+L1147</f>
+        <v>206</v>
+      </c>
+      <c r="N1147" s="30">
+        <f t="shared" ref="N1147:N1152" si="50">(L1147-K1147)*-1</f>
+        <v>12</v>
+      </c>
+      <c r="O1147" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1147" s="30">
+        <f t="shared" ref="P1147:P1152" si="51">IF(M1147&gt;I1147,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q1147" s="30" t="str">
+        <f t="shared" ref="Q1147:Q1152" si="52">IF(P1147=1,(M1147-I1147), "")</f>
+        <v/>
+      </c>
+      <c r="R1147" s="30">
+        <f t="shared" ref="R1147:R1152" si="53">IF(M1147&lt;I1147, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="S1147" s="30">
+        <f t="shared" ref="S1147:S1152" si="54">IF(R1147=1,(I1147-M1147),"")</f>
+        <v>10.5</v>
+      </c>
+      <c r="T1147" s="30">
+        <f t="shared" ref="T1147:T1152" si="55">IF(M1147=I1147,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1148" s="29">
+        <v>45750</v>
+      </c>
+      <c r="B1148" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1148" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1148" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1148" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1148" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1148" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1148" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1148" s="30">
+        <v>225.5</v>
+      </c>
+      <c r="J1148" s="31">
+        <v>11.5</v>
+      </c>
+      <c r="K1148" s="30">
+        <v>126</v>
+      </c>
+      <c r="L1148" s="30">
+        <v>113</v>
+      </c>
+      <c r="M1148" s="30">
+        <f t="shared" si="49"/>
+        <v>239</v>
+      </c>
+      <c r="N1148" s="30">
+        <f t="shared" si="50"/>
+        <v>13</v>
+      </c>
+      <c r="O1148" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1148" s="30">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1148" s="30">
+        <f t="shared" si="52"/>
+        <v>13.5</v>
+      </c>
+      <c r="R1148" s="30">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1148" s="30" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1148" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1149" s="29">
+        <v>45750</v>
+      </c>
+      <c r="B1149" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1149" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1149" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1149" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1149" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1149" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1149" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1149" s="30">
+        <v>226.5</v>
+      </c>
+      <c r="J1149" s="31">
+        <v>-2</v>
+      </c>
+      <c r="K1149" s="30">
+        <v>112</v>
+      </c>
+      <c r="L1149" s="30">
+        <v>103</v>
+      </c>
+      <c r="M1149" s="30">
+        <f t="shared" si="49"/>
+        <v>215</v>
+      </c>
+      <c r="N1149" s="30">
+        <f t="shared" si="50"/>
+        <v>9</v>
+      </c>
+      <c r="O1149" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1149" s="30">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1149" s="30" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1149" s="30">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1149" s="30">
+        <f t="shared" si="54"/>
+        <v>11.5</v>
+      </c>
+      <c r="T1149" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1150" s="29">
+        <v>45750</v>
+      </c>
+      <c r="B1150" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1150" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1150" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1150" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1150" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1150" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1150" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1150" s="30">
+        <v>225.5</v>
+      </c>
+      <c r="J1150" s="31">
+        <v>3.5</v>
+      </c>
+      <c r="K1150" s="30">
+        <v>110</v>
+      </c>
+      <c r="L1150" s="30">
+        <v>108</v>
+      </c>
+      <c r="M1150" s="30">
+        <f t="shared" si="49"/>
+        <v>218</v>
+      </c>
+      <c r="N1150" s="30">
+        <f t="shared" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="O1150" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1150" s="30">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1150" s="30" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1150" s="30">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1150" s="30">
+        <f t="shared" si="54"/>
+        <v>7.5</v>
+      </c>
+      <c r="T1150" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1151" s="29">
+        <v>45750</v>
+      </c>
+      <c r="B1151" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1151" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1151" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1151" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1151" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1151" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1151" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1151" s="30">
+        <v>217</v>
+      </c>
+      <c r="J1151" s="31">
+        <v>13.5</v>
+      </c>
+      <c r="K1151" s="30">
+        <v>105</v>
+      </c>
+      <c r="L1151" s="30">
+        <v>90</v>
+      </c>
+      <c r="M1151" s="30">
+        <f t="shared" si="49"/>
+        <v>195</v>
+      </c>
+      <c r="N1151" s="30">
+        <f t="shared" si="50"/>
+        <v>15</v>
+      </c>
+      <c r="O1151" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1151" s="30">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1151" s="30" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1151" s="30">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1151" s="30">
+        <f t="shared" si="54"/>
+        <v>22</v>
+      </c>
+      <c r="T1151" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1152" s="29">
+        <v>45750</v>
+      </c>
+      <c r="B1152" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1152" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1152" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1152" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1152" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1152" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1152" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1152" s="30">
+        <v>230</v>
+      </c>
+      <c r="J1152" s="31">
+        <v>-2</v>
+      </c>
+      <c r="K1152" s="30">
+        <v>123</v>
+      </c>
+      <c r="L1152" s="30">
+        <v>116</v>
+      </c>
+      <c r="M1152" s="30">
+        <f t="shared" si="49"/>
+        <v>239</v>
+      </c>
+      <c r="N1152" s="30">
+        <f t="shared" si="50"/>
+        <v>7</v>
+      </c>
+      <c r="O1152" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1152" s="30">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1152" s="30">
+        <f t="shared" si="52"/>
+        <v>9</v>
+      </c>
+      <c r="R1152" s="30">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1152" s="30" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1152" s="30">
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added game data for april 4 - april 8, 2025
</commit_message>
<xml_diff>
--- a/data/processed/nba_points_2024_2025.xlsx
+++ b/data/processed/nba_points_2024_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tyler/Documents/nba-points/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFA7929-00EE-3445-9DD3-00F1AE30E475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B007211-DE35-B14C-B98F-CBC98FDE5671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22940" yWindow="500" windowWidth="45860" windowHeight="28300" xr2:uid="{4B944735-6DC1-314A-AF10-68EBB82A81F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6928" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7156" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -1028,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78582E2E-5746-944D-860C-ACA920BD70CB}">
-  <dimension ref="A1:Y1152"/>
+  <dimension ref="A1:Y1190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1140" sqref="Q1140"/>
+      <pane ySplit="1" topLeftCell="A1147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1191" sqref="A1191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1207,19 +1207,19 @@
       </c>
       <c r="V2" s="7">
         <f>SUM(O:O)</f>
-        <v>1144</v>
+        <v>1182</v>
       </c>
       <c r="W2" s="12">
         <f>SUM(P:P)</f>
-        <v>595</v>
+        <v>614</v>
       </c>
       <c r="X2" s="15">
         <f>SUM(R:R)</f>
-        <v>547</v>
+        <v>565</v>
       </c>
       <c r="Y2" s="20">
         <f>SUM(T:T)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1370,15 +1370,15 @@
       </c>
       <c r="W4" s="14">
         <f>W2/V2</f>
-        <v>0.5201048951048951</v>
+        <v>0.51945854483925546</v>
       </c>
       <c r="X4" s="16">
         <f>X2/V2</f>
-        <v>0.47814685314685312</v>
+        <v>0.47800338409475468</v>
       </c>
       <c r="Y4" s="21">
         <f>Y2/V2</f>
-        <v>4.370629370629371E-3</v>
+        <v>5.076142131979695E-3</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1526,11 +1526,11 @@
       </c>
       <c r="W6" s="22">
         <f>AVERAGE(Q:Q)</f>
-        <v>14.920168067226891</v>
+        <v>14.894951140065146</v>
       </c>
       <c r="X6" s="23">
         <f>AVERAGE(S:S)</f>
-        <v>14.564899451553931</v>
+        <v>14.51504424778761</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -80137,34 +80137,34 @@
         <v>97</v>
       </c>
       <c r="M1147" s="30">
-        <f t="shared" ref="M1147:M1152" si="49">K1147+L1147</f>
+        <f t="shared" ref="M1147:M1190" si="49">K1147+L1147</f>
         <v>206</v>
       </c>
       <c r="N1147" s="30">
-        <f t="shared" ref="N1147:N1152" si="50">(L1147-K1147)*-1</f>
+        <f t="shared" ref="N1147:N1190" si="50">(L1147-K1147)*-1</f>
         <v>12</v>
       </c>
       <c r="O1147" s="30">
         <v>1</v>
       </c>
       <c r="P1147" s="30">
-        <f t="shared" ref="P1147:P1152" si="51">IF(M1147&gt;I1147,1,0)</f>
+        <f t="shared" ref="P1147:P1190" si="51">IF(M1147&gt;I1147,1,0)</f>
         <v>0</v>
       </c>
       <c r="Q1147" s="30" t="str">
-        <f t="shared" ref="Q1147:Q1152" si="52">IF(P1147=1,(M1147-I1147), "")</f>
+        <f t="shared" ref="Q1147:Q1190" si="52">IF(P1147=1,(M1147-I1147), "")</f>
         <v/>
       </c>
       <c r="R1147" s="30">
-        <f t="shared" ref="R1147:R1152" si="53">IF(M1147&lt;I1147, 1, 0)</f>
+        <f t="shared" ref="R1147:R1190" si="53">IF(M1147&lt;I1147, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="S1147" s="30">
-        <f t="shared" ref="S1147:S1152" si="54">IF(R1147=1,(I1147-M1147),"")</f>
+        <f t="shared" ref="S1147:S1190" si="54">IF(R1147=1,(I1147-M1147),"")</f>
         <v>10.5</v>
       </c>
       <c r="T1147" s="30">
-        <f t="shared" ref="T1147:T1152" si="55">IF(M1147=I1147,1,0)</f>
+        <f t="shared" ref="T1147:T1190" si="55">IF(M1147=I1147,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -80509,6 +80509,2628 @@
         <v/>
       </c>
       <c r="T1152" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1153" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1153" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1153" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1153" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1153" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1153" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1153" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1153" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1153" s="10">
+        <v>220.5</v>
+      </c>
+      <c r="J1153" s="11">
+        <v>10</v>
+      </c>
+      <c r="K1153" s="10">
+        <v>125</v>
+      </c>
+      <c r="L1153" s="10">
+        <v>102</v>
+      </c>
+      <c r="M1153" s="10">
+        <f t="shared" si="49"/>
+        <v>227</v>
+      </c>
+      <c r="N1153" s="10">
+        <f t="shared" si="50"/>
+        <v>23</v>
+      </c>
+      <c r="O1153" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1153" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1153" s="10">
+        <f t="shared" si="52"/>
+        <v>6.5</v>
+      </c>
+      <c r="R1153" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1153" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1153" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1154" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1154" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1154" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1154" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1154" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1154" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1154" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1154" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1154" s="10">
+        <v>237.5</v>
+      </c>
+      <c r="J1154" s="11">
+        <v>-15</v>
+      </c>
+      <c r="K1154" s="10">
+        <v>112</v>
+      </c>
+      <c r="L1154" s="10">
+        <v>140</v>
+      </c>
+      <c r="M1154" s="10">
+        <f t="shared" si="49"/>
+        <v>252</v>
+      </c>
+      <c r="N1154" s="10">
+        <f t="shared" si="50"/>
+        <v>-28</v>
+      </c>
+      <c r="O1154" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1154" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1154" s="10">
+        <f t="shared" si="52"/>
+        <v>14.5</v>
+      </c>
+      <c r="R1154" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1154" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1154" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1155" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1155" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1155" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1155" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1155" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1155" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1155" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1155" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1155" s="10">
+        <v>226</v>
+      </c>
+      <c r="J1155" s="11">
+        <v>-14.5</v>
+      </c>
+      <c r="K1155" s="10">
+        <v>103</v>
+      </c>
+      <c r="L1155" s="10">
+        <v>123</v>
+      </c>
+      <c r="M1155" s="10">
+        <f t="shared" si="49"/>
+        <v>226</v>
+      </c>
+      <c r="N1155" s="10">
+        <f t="shared" si="50"/>
+        <v>-20</v>
+      </c>
+      <c r="O1155" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1155" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1155" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1155" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1155" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1155" s="10">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1156" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1156" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1156" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1156" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1156" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1156" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1156" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1156" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1156" s="10">
+        <v>231.5</v>
+      </c>
+      <c r="J1156" s="11">
+        <v>9.5</v>
+      </c>
+      <c r="K1156" s="10">
+        <v>117</v>
+      </c>
+      <c r="L1156" s="10">
+        <v>105</v>
+      </c>
+      <c r="M1156" s="10">
+        <f t="shared" si="49"/>
+        <v>222</v>
+      </c>
+      <c r="N1156" s="10">
+        <f t="shared" si="50"/>
+        <v>12</v>
+      </c>
+      <c r="O1156" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1156" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1156" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1156" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1156" s="10">
+        <f t="shared" si="54"/>
+        <v>9.5</v>
+      </c>
+      <c r="T1156" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1157" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1157" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1157" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1157" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1157" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1157" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1157" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1157" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1157" s="10">
+        <v>241.5</v>
+      </c>
+      <c r="J1157" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K1157" s="10">
+        <v>113</v>
+      </c>
+      <c r="L1157" s="10">
+        <v>118</v>
+      </c>
+      <c r="M1157" s="10">
+        <f t="shared" si="49"/>
+        <v>231</v>
+      </c>
+      <c r="N1157" s="10">
+        <f t="shared" si="50"/>
+        <v>-5</v>
+      </c>
+      <c r="O1157" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1157" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1157" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1157" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1157" s="10">
+        <f t="shared" si="54"/>
+        <v>10.5</v>
+      </c>
+      <c r="T1157" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1158" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1158" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1158" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1158" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1158" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1158" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1158" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1158" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1158" s="10">
+        <v>240.5</v>
+      </c>
+      <c r="J1158" s="11">
+        <v>14.5</v>
+      </c>
+      <c r="K1158" s="10">
+        <v>114</v>
+      </c>
+      <c r="L1158" s="10">
+        <v>113</v>
+      </c>
+      <c r="M1158" s="10">
+        <f t="shared" si="49"/>
+        <v>227</v>
+      </c>
+      <c r="N1158" s="10">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="O1158" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1158" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1158" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1158" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1158" s="10">
+        <f t="shared" si="54"/>
+        <v>13.5</v>
+      </c>
+      <c r="T1158" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1159" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1159" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1159" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1159" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1159" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1159" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1159" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1159" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1159" s="10">
+        <v>228.5</v>
+      </c>
+      <c r="J1159" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="K1159" s="10">
+        <v>111</v>
+      </c>
+      <c r="L1159" s="10">
+        <v>125</v>
+      </c>
+      <c r="M1159" s="10">
+        <f t="shared" si="49"/>
+        <v>236</v>
+      </c>
+      <c r="N1159" s="10">
+        <f t="shared" si="50"/>
+        <v>-14</v>
+      </c>
+      <c r="O1159" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1159" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1159" s="10">
+        <f t="shared" si="52"/>
+        <v>7.5</v>
+      </c>
+      <c r="R1159" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1159" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1159" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1160" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1160" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1160" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1160" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1160" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1160" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1160" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1160" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1160" s="10">
+        <v>234.5</v>
+      </c>
+      <c r="J1160" s="11">
+        <v>-1.5</v>
+      </c>
+      <c r="K1160" s="10">
+        <v>104</v>
+      </c>
+      <c r="L1160" s="10">
+        <v>118</v>
+      </c>
+      <c r="M1160" s="10">
+        <f t="shared" si="49"/>
+        <v>222</v>
+      </c>
+      <c r="N1160" s="10">
+        <f t="shared" si="50"/>
+        <v>-14</v>
+      </c>
+      <c r="O1160" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1160" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1160" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1160" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1160" s="10">
+        <f t="shared" si="54"/>
+        <v>12.5</v>
+      </c>
+      <c r="T1160" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1161" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1161" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1161" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1161" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1161" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1161" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1161" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1161" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1161" s="10">
+        <v>225.5</v>
+      </c>
+      <c r="J1161" s="11">
+        <v>-5</v>
+      </c>
+      <c r="K1161" s="10">
+        <v>91</v>
+      </c>
+      <c r="L1161" s="10">
+        <v>114</v>
+      </c>
+      <c r="M1161" s="10">
+        <f t="shared" si="49"/>
+        <v>205</v>
+      </c>
+      <c r="N1161" s="10">
+        <f t="shared" si="50"/>
+        <v>-23</v>
+      </c>
+      <c r="O1161" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1161" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1161" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1161" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1161" s="10">
+        <f t="shared" si="54"/>
+        <v>20.5</v>
+      </c>
+      <c r="T1161" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1162" s="9">
+        <v>45751</v>
+      </c>
+      <c r="B1162" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1162" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1162" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1162" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1162" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1162" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1162" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1162" s="10">
+        <v>222.5</v>
+      </c>
+      <c r="J1162" s="11">
+        <v>-14</v>
+      </c>
+      <c r="K1162" s="10">
+        <v>108</v>
+      </c>
+      <c r="L1162" s="10">
+        <v>124</v>
+      </c>
+      <c r="M1162" s="10">
+        <f t="shared" si="49"/>
+        <v>232</v>
+      </c>
+      <c r="N1162" s="10">
+        <f t="shared" si="50"/>
+        <v>-16</v>
+      </c>
+      <c r="O1162" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1162" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1162" s="10">
+        <f t="shared" si="52"/>
+        <v>9.5</v>
+      </c>
+      <c r="R1162" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1162" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1162" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1163" s="29">
+        <v>45752</v>
+      </c>
+      <c r="B1163" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1163" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1163" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1163" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1163" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1163" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1163" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1163" s="30">
+        <v>234</v>
+      </c>
+      <c r="J1163" s="31">
+        <v>3</v>
+      </c>
+      <c r="K1163" s="30">
+        <v>121</v>
+      </c>
+      <c r="L1163" s="30">
+        <v>105</v>
+      </c>
+      <c r="M1163" s="30">
+        <f t="shared" si="49"/>
+        <v>226</v>
+      </c>
+      <c r="N1163" s="30">
+        <f t="shared" si="50"/>
+        <v>16</v>
+      </c>
+      <c r="O1163" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1163" s="30">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1163" s="30" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1163" s="30">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1163" s="30">
+        <f t="shared" si="54"/>
+        <v>8</v>
+      </c>
+      <c r="T1163" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1164" s="29">
+        <v>45752</v>
+      </c>
+      <c r="B1164" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1164" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1164" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1164" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1164" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1164" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1164" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1164" s="30">
+        <v>225.5</v>
+      </c>
+      <c r="J1164" s="31">
+        <v>14.5</v>
+      </c>
+      <c r="K1164" s="30">
+        <v>114</v>
+      </c>
+      <c r="L1164" s="30">
+        <v>109</v>
+      </c>
+      <c r="M1164" s="30">
+        <f t="shared" si="49"/>
+        <v>223</v>
+      </c>
+      <c r="N1164" s="30">
+        <f t="shared" si="50"/>
+        <v>5</v>
+      </c>
+      <c r="O1164" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1164" s="30">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1164" s="30" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1164" s="30">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1164" s="30">
+        <f t="shared" si="54"/>
+        <v>2.5</v>
+      </c>
+      <c r="T1164" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1165" s="29">
+        <v>45752</v>
+      </c>
+      <c r="B1165" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1165" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1165" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1165" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1165" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1165" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1165" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1165" s="30">
+        <v>239.5</v>
+      </c>
+      <c r="J1165" s="31">
+        <v>-1.5</v>
+      </c>
+      <c r="K1165" s="30">
+        <v>109</v>
+      </c>
+      <c r="L1165" s="30">
+        <v>103</v>
+      </c>
+      <c r="M1165" s="30">
+        <f t="shared" si="49"/>
+        <v>212</v>
+      </c>
+      <c r="N1165" s="30">
+        <f t="shared" si="50"/>
+        <v>6</v>
+      </c>
+      <c r="O1165" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1165" s="30">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1165" s="30" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1165" s="30">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1165" s="30">
+        <f t="shared" si="54"/>
+        <v>27.5</v>
+      </c>
+      <c r="T1165" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1166" s="29">
+        <v>45752</v>
+      </c>
+      <c r="B1166" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1166" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1166" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1166" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1166" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1166" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1166" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1166" s="30">
+        <v>215</v>
+      </c>
+      <c r="J1166" s="31">
+        <v>1</v>
+      </c>
+      <c r="K1166" s="30">
+        <v>121</v>
+      </c>
+      <c r="L1166" s="30">
+        <v>115</v>
+      </c>
+      <c r="M1166" s="30">
+        <f t="shared" si="49"/>
+        <v>236</v>
+      </c>
+      <c r="N1166" s="30">
+        <f t="shared" si="50"/>
+        <v>6</v>
+      </c>
+      <c r="O1166" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1166" s="30">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1166" s="30">
+        <f t="shared" si="52"/>
+        <v>21</v>
+      </c>
+      <c r="R1166" s="30">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1166" s="30" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1166" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1167" s="29">
+        <v>45752</v>
+      </c>
+      <c r="B1167" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1167" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1167" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1167" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1167" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1167" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1167" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1167" s="30">
+        <v>224.5</v>
+      </c>
+      <c r="J1167" s="31">
+        <v>-9.5</v>
+      </c>
+      <c r="K1167" s="30">
+        <v>104</v>
+      </c>
+      <c r="L1167" s="30">
+        <v>135</v>
+      </c>
+      <c r="M1167" s="30">
+        <f t="shared" si="49"/>
+        <v>239</v>
+      </c>
+      <c r="N1167" s="30">
+        <f t="shared" si="50"/>
+        <v>-31</v>
+      </c>
+      <c r="O1167" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1167" s="30">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1167" s="30">
+        <f t="shared" si="52"/>
+        <v>14.5</v>
+      </c>
+      <c r="R1167" s="30">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1167" s="30" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1167" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1168" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1168" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1168" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1168" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1168" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1168" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1168" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1168" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1168" s="10">
+        <v>227.5</v>
+      </c>
+      <c r="J1168" s="11">
+        <v>8.5</v>
+      </c>
+      <c r="K1168" s="10">
+        <v>131</v>
+      </c>
+      <c r="L1168" s="10">
+        <v>117</v>
+      </c>
+      <c r="M1168" s="10">
+        <f t="shared" si="49"/>
+        <v>248</v>
+      </c>
+      <c r="N1168" s="10">
+        <f t="shared" si="50"/>
+        <v>14</v>
+      </c>
+      <c r="O1168" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1168" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1168" s="10">
+        <f t="shared" si="52"/>
+        <v>20.5</v>
+      </c>
+      <c r="R1168" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1168" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1168" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1169" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1169" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1169" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1169" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1169" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1169" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1169" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1169" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1169" s="10">
+        <v>216</v>
+      </c>
+      <c r="J1169" s="11">
+        <v>2</v>
+      </c>
+      <c r="K1169" s="10">
+        <v>120</v>
+      </c>
+      <c r="L1169" s="10">
+        <v>109</v>
+      </c>
+      <c r="M1169" s="10">
+        <f t="shared" si="49"/>
+        <v>229</v>
+      </c>
+      <c r="N1169" s="10">
+        <f t="shared" si="50"/>
+        <v>11</v>
+      </c>
+      <c r="O1169" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1169" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1169" s="10">
+        <f t="shared" si="52"/>
+        <v>13</v>
+      </c>
+      <c r="R1169" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1169" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1169" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1170" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1170" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1170" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1170" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1170" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1170" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1170" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1170" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1170" s="10">
+        <v>233.5</v>
+      </c>
+      <c r="J1170" s="11">
+        <v>-9.5</v>
+      </c>
+      <c r="K1170" s="10">
+        <v>126</v>
+      </c>
+      <c r="L1170" s="10">
+        <v>99</v>
+      </c>
+      <c r="M1170" s="10">
+        <f t="shared" si="49"/>
+        <v>225</v>
+      </c>
+      <c r="N1170" s="10">
+        <f t="shared" si="50"/>
+        <v>27</v>
+      </c>
+      <c r="O1170" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1170" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1170" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1170" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1170" s="10">
+        <f t="shared" si="54"/>
+        <v>8.5</v>
+      </c>
+      <c r="T1170" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1171" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1171" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1171" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1171" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1171" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1171" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1171" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1171" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1171" s="10">
+        <v>228.5</v>
+      </c>
+      <c r="J1171" s="11">
+        <v>-19.5</v>
+      </c>
+      <c r="K1171" s="10">
+        <v>90</v>
+      </c>
+      <c r="L1171" s="10">
+        <v>124</v>
+      </c>
+      <c r="M1171" s="10">
+        <f t="shared" si="49"/>
+        <v>214</v>
+      </c>
+      <c r="N1171" s="10">
+        <f t="shared" si="50"/>
+        <v>-34</v>
+      </c>
+      <c r="O1171" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1171" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1171" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1171" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1171" s="10">
+        <f t="shared" si="54"/>
+        <v>14.5</v>
+      </c>
+      <c r="T1171" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1172" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1172" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1172" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1172" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1172" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1172" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1172" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1172" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1172" s="10">
+        <v>235.5</v>
+      </c>
+      <c r="J1172" s="11">
+        <v>-9.5</v>
+      </c>
+      <c r="K1172" s="10">
+        <v>120</v>
+      </c>
+      <c r="L1172" s="10">
+        <v>113</v>
+      </c>
+      <c r="M1172" s="10">
+        <f t="shared" si="49"/>
+        <v>233</v>
+      </c>
+      <c r="N1172" s="10">
+        <f t="shared" si="50"/>
+        <v>7</v>
+      </c>
+      <c r="O1172" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1172" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1172" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1172" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1172" s="10">
+        <f t="shared" si="54"/>
+        <v>2.5</v>
+      </c>
+      <c r="T1172" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1173" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1173" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1173" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1173" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1173" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1173" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1173" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1173" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1173" s="10">
+        <v>239.5</v>
+      </c>
+      <c r="J1173" s="11">
+        <v>-12.5</v>
+      </c>
+      <c r="K1173" s="10">
+        <v>134</v>
+      </c>
+      <c r="L1173" s="10">
+        <v>147</v>
+      </c>
+      <c r="M1173" s="10">
+        <f t="shared" si="49"/>
+        <v>281</v>
+      </c>
+      <c r="N1173" s="10">
+        <f t="shared" si="50"/>
+        <v>-13</v>
+      </c>
+      <c r="O1173" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1173" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1173" s="10">
+        <f t="shared" si="52"/>
+        <v>41.5</v>
+      </c>
+      <c r="R1173" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1173" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1173" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1174" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1174" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1174" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1174" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1174" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1174" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1174" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1174" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1174" s="10">
+        <v>228.5</v>
+      </c>
+      <c r="J1174" s="11">
+        <v>-4</v>
+      </c>
+      <c r="K1174" s="10">
+        <v>109</v>
+      </c>
+      <c r="L1174" s="10">
+        <v>120</v>
+      </c>
+      <c r="M1174" s="10">
+        <f t="shared" si="49"/>
+        <v>229</v>
+      </c>
+      <c r="N1174" s="10">
+        <f t="shared" si="50"/>
+        <v>-11</v>
+      </c>
+      <c r="O1174" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1174" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1174" s="10">
+        <f t="shared" si="52"/>
+        <v>0.5</v>
+      </c>
+      <c r="R1174" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1174" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1174" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1175" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1175" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1175" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1175" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1175" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1175" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1175" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1175" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1175" s="10">
+        <v>225.5</v>
+      </c>
+      <c r="J1175" s="11">
+        <v>-7.5</v>
+      </c>
+      <c r="K1175" s="10">
+        <v>98</v>
+      </c>
+      <c r="L1175" s="10">
+        <v>112</v>
+      </c>
+      <c r="M1175" s="10">
+        <f t="shared" si="49"/>
+        <v>210</v>
+      </c>
+      <c r="N1175" s="10">
+        <f t="shared" si="50"/>
+        <v>-14</v>
+      </c>
+      <c r="O1175" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1175" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1175" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1175" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1175" s="10">
+        <f t="shared" si="54"/>
+        <v>15.5</v>
+      </c>
+      <c r="T1175" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1176" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1176" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1176" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1176" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1176" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1176" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1176" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1176" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1176" s="10">
+        <v>237.5</v>
+      </c>
+      <c r="J1176" s="11">
+        <v>-4</v>
+      </c>
+      <c r="K1176" s="10">
+        <v>125</v>
+      </c>
+      <c r="L1176" s="10">
+        <v>120</v>
+      </c>
+      <c r="M1176" s="10">
+        <f t="shared" si="49"/>
+        <v>245</v>
+      </c>
+      <c r="N1176" s="10">
+        <f t="shared" si="50"/>
+        <v>5</v>
+      </c>
+      <c r="O1176" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1176" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1176" s="10">
+        <f t="shared" si="52"/>
+        <v>7.5</v>
+      </c>
+      <c r="R1176" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1176" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1176" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1177" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1177" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1177" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1177" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1177" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1177" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1177" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1177" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1177" s="10">
+        <v>227.5</v>
+      </c>
+      <c r="J1177" s="11">
+        <v>-3</v>
+      </c>
+      <c r="K1177" s="10">
+        <v>106</v>
+      </c>
+      <c r="L1177" s="10">
+        <v>96</v>
+      </c>
+      <c r="M1177" s="10">
+        <f t="shared" si="49"/>
+        <v>202</v>
+      </c>
+      <c r="N1177" s="10">
+        <f t="shared" si="50"/>
+        <v>10</v>
+      </c>
+      <c r="O1177" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1177" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1177" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1177" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1177" s="10">
+        <f t="shared" si="54"/>
+        <v>25.5</v>
+      </c>
+      <c r="T1177" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1178" s="9">
+        <v>45753</v>
+      </c>
+      <c r="B1178" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1178" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1178" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1178" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1178" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1178" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1178" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1178" s="10">
+        <v>226</v>
+      </c>
+      <c r="J1178" s="11">
+        <v>10.5</v>
+      </c>
+      <c r="K1178" s="10">
+        <v>111</v>
+      </c>
+      <c r="L1178" s="10">
+        <v>107</v>
+      </c>
+      <c r="M1178" s="10">
+        <f t="shared" si="49"/>
+        <v>218</v>
+      </c>
+      <c r="N1178" s="10">
+        <f t="shared" si="50"/>
+        <v>4</v>
+      </c>
+      <c r="O1178" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1178" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1178" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1178" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1178" s="10">
+        <f t="shared" si="54"/>
+        <v>8</v>
+      </c>
+      <c r="T1178" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1179" s="29">
+        <v>45754</v>
+      </c>
+      <c r="B1179" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1179" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1179" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1179" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1179" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1179" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1179" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1179" s="30">
+        <v>228.5</v>
+      </c>
+      <c r="J1179" s="31">
+        <v>-6.5</v>
+      </c>
+      <c r="K1179" s="30">
+        <v>127</v>
+      </c>
+      <c r="L1179" s="30">
+        <v>117</v>
+      </c>
+      <c r="M1179" s="30">
+        <f t="shared" si="49"/>
+        <v>244</v>
+      </c>
+      <c r="N1179" s="30">
+        <f t="shared" si="50"/>
+        <v>10</v>
+      </c>
+      <c r="O1179" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1179" s="30">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1179" s="30">
+        <f t="shared" si="52"/>
+        <v>15.5</v>
+      </c>
+      <c r="R1179" s="30">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1179" s="30" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1179" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1180" s="29">
+        <v>45754</v>
+      </c>
+      <c r="B1180" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1180" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1180" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1180" s="30">
+        <v>0</v>
+      </c>
+      <c r="F1180" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1180" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1180" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1180" s="30">
+        <v>213</v>
+      </c>
+      <c r="J1180" s="31">
+        <v>-12</v>
+      </c>
+      <c r="K1180" s="30">
+        <v>105</v>
+      </c>
+      <c r="L1180" s="30">
+        <v>117</v>
+      </c>
+      <c r="M1180" s="30">
+        <f t="shared" si="49"/>
+        <v>222</v>
+      </c>
+      <c r="N1180" s="30">
+        <f t="shared" si="50"/>
+        <v>-12</v>
+      </c>
+      <c r="O1180" s="30">
+        <v>1</v>
+      </c>
+      <c r="P1180" s="30">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1180" s="30">
+        <f t="shared" si="52"/>
+        <v>9</v>
+      </c>
+      <c r="R1180" s="30">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1180" s="30" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1180" s="30">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1181" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1181" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1181" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1181" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1181" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1181" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1181" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1181" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1181" s="10">
+        <v>238.5</v>
+      </c>
+      <c r="J1181" s="11">
+        <v>-9</v>
+      </c>
+      <c r="K1181" s="10">
+        <v>113</v>
+      </c>
+      <c r="L1181" s="10">
+        <v>135</v>
+      </c>
+      <c r="M1181" s="10">
+        <f t="shared" si="49"/>
+        <v>248</v>
+      </c>
+      <c r="N1181" s="10">
+        <f t="shared" si="50"/>
+        <v>-22</v>
+      </c>
+      <c r="O1181" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1181" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1181" s="10">
+        <f t="shared" si="52"/>
+        <v>9.5</v>
+      </c>
+      <c r="R1181" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1181" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1181" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1182" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1182" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1182" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1182" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1182" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1182" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1182" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1182" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1182" s="10">
+        <v>225</v>
+      </c>
+      <c r="J1182" s="11">
+        <v>-4.5</v>
+      </c>
+      <c r="K1182" s="10">
+        <v>112</v>
+      </c>
+      <c r="L1182" s="10">
+        <v>119</v>
+      </c>
+      <c r="M1182" s="10">
+        <f t="shared" si="49"/>
+        <v>231</v>
+      </c>
+      <c r="N1182" s="10">
+        <f t="shared" si="50"/>
+        <v>-7</v>
+      </c>
+      <c r="O1182" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1182" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1182" s="10">
+        <f t="shared" si="52"/>
+        <v>6</v>
+      </c>
+      <c r="R1182" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1182" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1182" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1183" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1183" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1183" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1183" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1183" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1183" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1183" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1183" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1183" s="10">
+        <v>238.5</v>
+      </c>
+      <c r="J1183" s="11">
+        <v>-18.5</v>
+      </c>
+      <c r="K1183" s="10">
+        <v>98</v>
+      </c>
+      <c r="L1183" s="10">
+        <v>104</v>
+      </c>
+      <c r="M1183" s="10">
+        <f t="shared" si="49"/>
+        <v>202</v>
+      </c>
+      <c r="N1183" s="10">
+        <f t="shared" si="50"/>
+        <v>-6</v>
+      </c>
+      <c r="O1183" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1183" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1183" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1183" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1183" s="10">
+        <f t="shared" si="54"/>
+        <v>36.5</v>
+      </c>
+      <c r="T1183" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1184" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1184" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1184" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1184" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1184" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1184" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1184" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1184" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1184" s="10">
+        <v>230</v>
+      </c>
+      <c r="J1184" s="11">
+        <v>13.5</v>
+      </c>
+      <c r="K1184" s="10">
+        <v>124</v>
+      </c>
+      <c r="L1184" s="10">
+        <v>100</v>
+      </c>
+      <c r="M1184" s="10">
+        <f t="shared" si="49"/>
+        <v>224</v>
+      </c>
+      <c r="N1184" s="10">
+        <f t="shared" si="50"/>
+        <v>24</v>
+      </c>
+      <c r="O1184" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1184" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1184" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1184" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1184" s="10">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="T1184" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1185" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1185" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1185" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1185" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1185" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1185" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1185" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1185" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1185" s="10">
+        <v>214</v>
+      </c>
+      <c r="J1185" s="11">
+        <v>-2</v>
+      </c>
+      <c r="K1185" s="10">
+        <v>114</v>
+      </c>
+      <c r="L1185" s="10">
+        <v>119</v>
+      </c>
+      <c r="M1185" s="10">
+        <f t="shared" si="49"/>
+        <v>233</v>
+      </c>
+      <c r="N1185" s="10">
+        <f t="shared" si="50"/>
+        <v>-5</v>
+      </c>
+      <c r="O1185" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1185" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1185" s="10">
+        <f t="shared" si="52"/>
+        <v>19</v>
+      </c>
+      <c r="R1185" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1185" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1185" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1186" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1186" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1186" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1186" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1186" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1186" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1186" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1186" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1186" s="10">
+        <v>223.5</v>
+      </c>
+      <c r="J1186" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="K1186" s="10">
+        <v>119</v>
+      </c>
+      <c r="L1186" s="10">
+        <v>117</v>
+      </c>
+      <c r="M1186" s="10">
+        <f t="shared" si="49"/>
+        <v>236</v>
+      </c>
+      <c r="N1186" s="10">
+        <f t="shared" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="O1186" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1186" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1186" s="10">
+        <f t="shared" si="52"/>
+        <v>12.5</v>
+      </c>
+      <c r="R1186" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1186" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1186" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1187" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1187" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1187" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1187" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1187" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1187" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1187" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1187" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1187" s="10">
+        <v>225</v>
+      </c>
+      <c r="J1187" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="K1187" s="10">
+        <v>103</v>
+      </c>
+      <c r="L1187" s="10">
+        <v>110</v>
+      </c>
+      <c r="M1187" s="10">
+        <f t="shared" si="49"/>
+        <v>213</v>
+      </c>
+      <c r="N1187" s="10">
+        <f t="shared" si="50"/>
+        <v>-7</v>
+      </c>
+      <c r="O1187" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1187" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1187" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1187" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1187" s="10">
+        <f t="shared" si="54"/>
+        <v>12</v>
+      </c>
+      <c r="T1187" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1188" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1188" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1188" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1188" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1188" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1188" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1188" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1188" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1188" s="10">
+        <v>229.5</v>
+      </c>
+      <c r="J1188" s="11">
+        <v>-8.5</v>
+      </c>
+      <c r="K1188" s="10">
+        <v>120</v>
+      </c>
+      <c r="L1188" s="10">
+        <v>136</v>
+      </c>
+      <c r="M1188" s="10">
+        <f t="shared" si="49"/>
+        <v>256</v>
+      </c>
+      <c r="N1188" s="10">
+        <f t="shared" si="50"/>
+        <v>-16</v>
+      </c>
+      <c r="O1188" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1188" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1188" s="10">
+        <f t="shared" si="52"/>
+        <v>26.5</v>
+      </c>
+      <c r="R1188" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1188" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1188" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1189" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1189" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1189" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1189" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1189" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1189" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1189" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1189" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1189" s="10">
+        <v>228.5</v>
+      </c>
+      <c r="J1189" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="K1189" s="10">
+        <v>133</v>
+      </c>
+      <c r="L1189" s="10">
+        <v>95</v>
+      </c>
+      <c r="M1189" s="10">
+        <f t="shared" si="49"/>
+        <v>228</v>
+      </c>
+      <c r="N1189" s="10">
+        <f t="shared" si="50"/>
+        <v>38</v>
+      </c>
+      <c r="O1189" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1189" s="10">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q1189" s="10" t="str">
+        <f t="shared" si="52"/>
+        <v/>
+      </c>
+      <c r="R1189" s="10">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S1189" s="10">
+        <f t="shared" si="54"/>
+        <v>0.5</v>
+      </c>
+      <c r="T1189" s="10">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1190" s="9">
+        <v>45755</v>
+      </c>
+      <c r="B1190" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1190" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1190" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1190" s="10">
+        <v>0</v>
+      </c>
+      <c r="F1190" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1190" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1190" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1190" s="10">
+        <v>225.5</v>
+      </c>
+      <c r="J1190" s="11">
+        <v>-14</v>
+      </c>
+      <c r="K1190" s="10">
+        <v>117</v>
+      </c>
+      <c r="L1190" s="10">
+        <v>122</v>
+      </c>
+      <c r="M1190" s="10">
+        <f t="shared" si="49"/>
+        <v>239</v>
+      </c>
+      <c r="N1190" s="10">
+        <f t="shared" si="50"/>
+        <v>-5</v>
+      </c>
+      <c r="O1190" s="10">
+        <v>1</v>
+      </c>
+      <c r="P1190" s="10">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="Q1190" s="10">
+        <f t="shared" si="52"/>
+        <v>13.5</v>
+      </c>
+      <c r="R1190" s="10">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S1190" s="10" t="str">
+        <f t="shared" si="54"/>
+        <v/>
+      </c>
+      <c r="T1190" s="10">
         <f t="shared" si="55"/>
         <v>0</v>
       </c>

</xml_diff>